<commit_message>
student and course collection complete
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B6A5B40-C307-4461-86FF-13AAB95B3753}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFF0AD2-DED4-4AA6-A6B5-FFC5BE42915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="64">
   <si>
     <t>Student Table</t>
   </si>
@@ -192,10 +192,31 @@
     <t>Department Name</t>
   </si>
   <si>
-    <t>Year</t>
-  </si>
-  <si>
     <t xml:space="preserve">student id   </t>
+  </si>
+  <si>
+    <t>Prerequisities</t>
+  </si>
+  <si>
+    <t>Department Head</t>
+  </si>
+  <si>
+    <t>Office Manager</t>
+  </si>
+  <si>
+    <t>Professors</t>
+  </si>
+  <si>
+    <t>Associate Professors</t>
+  </si>
+  <si>
+    <t>Assistant Professors</t>
+  </si>
+  <si>
+    <t>Lecturers</t>
+  </si>
+  <si>
+    <t>Number of students</t>
   </si>
 </sst>
 </file>
@@ -211,12 +232,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -231,11 +258,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -516,15 +544,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.5546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="25.77734375" bestFit="1" customWidth="1"/>
@@ -715,7 +743,7 @@
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B15" t="s">
         <v>40</v>
@@ -772,7 +800,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
+      <c r="A23" s="2" t="s">
         <v>53</v>
       </c>
       <c r="B23" t="s">
@@ -780,8 +808,8 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>55</v>
+      <c r="A24" s="2" t="s">
+        <v>56</v>
       </c>
       <c r="B24" t="s">
         <v>46</v>
@@ -799,12 +827,42 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>55</v>
+        <v>58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
lecturer collection populated with colleges
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EFF0AD2-DED4-4AA6-A6B5-FFC5BE42915D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A6A0A0A-685E-4C1F-A468-5272A9073EF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="108" yWindow="0" windowWidth="11712" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -260,10 +260,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -547,7 +547,7 @@
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="E12" sqref="D12:E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -564,18 +564,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="D1" s="1" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="E1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -800,7 +800,7 @@
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="1" t="s">
         <v>53</v>
       </c>
       <c r="B23" t="s">
@@ -808,7 +808,7 @@
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B24" t="s">

</xml_diff>

<commit_message>
enroll students in courses and electives
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44EE17A0-DA2E-42C0-AE04-B6E938CDD962}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC53A49B-4CE2-4978-B565-00701AC145FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="108" yWindow="0" windowWidth="11712" windowHeight="12960" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -535,8 +535,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A21"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
create advisors and assign student advisors
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC53A49B-4CE2-4978-B565-00701AC145FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{961ADB20-E06F-4EDF-A34F-12E21C24DB11}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="57">
   <si>
     <t>Student Table</t>
   </si>
@@ -180,18 +180,12 @@
     <t>Version 2</t>
   </si>
   <si>
-    <t>Semester</t>
-  </si>
-  <si>
     <t>Department Name</t>
   </si>
   <si>
     <t xml:space="preserve">student id   </t>
   </si>
   <si>
-    <t>Prerequisities</t>
-  </si>
-  <si>
     <t>Department Head</t>
   </si>
   <si>
@@ -199,6 +193,9 @@
   </si>
   <si>
     <t>Faculty</t>
+  </si>
+  <si>
+    <t>Students</t>
   </si>
 </sst>
 </file>
@@ -214,18 +211,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -249,10 +240,10 @@
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -535,8 +526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,18 +544,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="2"/>
+      <c r="D1" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="E1" s="2"/>
+      <c r="G1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="2"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
@@ -587,10 +578,10 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D3" t="s">
@@ -607,10 +598,10 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D4" t="s">
@@ -627,10 +618,10 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>16</v>
       </c>
       <c r="D5" t="s">
@@ -647,18 +638,18 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D7" t="s">
@@ -666,10 +657,10 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D8" t="s">
@@ -677,10 +668,10 @@
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D9" t="s">
@@ -688,10 +679,10 @@
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D10" t="s">
@@ -699,10 +690,10 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D11" t="s">
@@ -710,36 +701,36 @@
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" t="s">
+      <c r="B13" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B15" t="s">
-        <v>38</v>
+      <c r="A15" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B16" t="s">
+      <c r="B16" s="1" t="s">
         <v>47</v>
       </c>
     </row>
@@ -749,7 +740,7 @@
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="2" t="s">
+      <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
       <c r="B18" t="s">
@@ -757,7 +748,7 @@
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
       <c r="B19" t="s">
@@ -765,7 +756,7 @@
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B20" t="s">
@@ -773,7 +764,7 @@
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="B21" t="s">
@@ -781,17 +772,13 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="1" t="s">
-        <v>51</v>
-      </c>
+      <c r="A22" s="3"/>
       <c r="B22" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>54</v>
-      </c>
+      <c r="A23" s="3"/>
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -801,34 +788,39 @@
         <v>44</v>
       </c>
     </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="B25" t="s">
+        <v>20</v>
+      </c>
+    </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>52</v>
+      <c r="A27" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>56</v>
+      <c r="A31" s="1" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update electives with instructor ratings
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CA024A-AF6E-43C1-B17C-6916DD005032}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3CB97D-BBC5-4721-90DB-64632A70F638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -229,7 +229,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -239,6 +239,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -255,12 +261,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -544,7 +551,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -666,7 +673,7 @@
       <c r="B7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -677,7 +684,7 @@
       <c r="B8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3" t="s">
         <v>27</v>
       </c>
     </row>
@@ -688,7 +695,7 @@
       <c r="B9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D9" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -699,7 +706,7 @@
       <c r="B10" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="D10" t="s">
+      <c r="D10" s="3" t="s">
         <v>32</v>
       </c>
     </row>
@@ -710,7 +717,7 @@
       <c r="B11" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D11" s="3" t="s">
         <v>33</v>
       </c>
     </row>
@@ -718,7 +725,7 @@
       <c r="A12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="1" t="s">
         <v>62</v>
       </c>
     </row>
@@ -744,7 +751,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+      <c r="A16" s="1" t="s">
         <v>61</v>
       </c>
       <c r="B16" s="1" t="s">

</xml_diff>

<commit_message>
Updated schema for accounts
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F3CB97D-BBC5-4721-90DB-64632A70F638}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAE6E23-8CCF-43D0-A58B-1BD826C3AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="65">
   <si>
     <t>Student Table</t>
   </si>
@@ -57,18 +57,12 @@
     <t>Student ID number</t>
   </si>
   <si>
-    <t>Student Id</t>
-  </si>
-  <si>
     <t>Financial aid</t>
   </si>
   <si>
     <t>Financial aid amount</t>
   </si>
   <si>
-    <t>Balance</t>
-  </si>
-  <si>
     <t>Degree Type</t>
   </si>
   <si>
@@ -135,9 +129,6 @@
     <t>Advisor ID</t>
   </si>
   <si>
-    <t>Student id</t>
-  </si>
-  <si>
     <t>Housing</t>
   </si>
   <si>
@@ -147,9 +138,6 @@
     <t>Accounts</t>
   </si>
   <si>
-    <t>Total Tuition</t>
-  </si>
-  <si>
     <t>Advisor name</t>
   </si>
   <si>
@@ -214,6 +202,24 @@
   </si>
   <si>
     <t>Rating</t>
+  </si>
+  <si>
+    <t>student_id</t>
+  </si>
+  <si>
+    <t>balance</t>
+  </si>
+  <si>
+    <t>financial aid</t>
+  </si>
+  <si>
+    <t>student(s)</t>
+  </si>
+  <si>
+    <t>housing</t>
+  </si>
+  <si>
+    <t>tuition</t>
   </si>
 </sst>
 </file>
@@ -261,13 +267,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,7 +558,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -568,37 +575,37 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="2"/>
-      <c r="D1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" s="2"/>
-      <c r="G1" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="H1" s="2"/>
+      <c r="A1" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="D1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E1" s="3"/>
+      <c r="G1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" t="s">
         <v>28</v>
       </c>
-      <c r="E2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
       <c r="H2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -609,16 +616,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G3" t="s">
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -629,16 +636,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H4" t="s">
-        <v>13</v>
+        <v>53</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -646,16 +653,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H5" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -663,18 +670,24 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
+      </c>
+      <c r="H6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>31</v>
+        <v>16</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -682,10 +695,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -693,10 +706,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>26</v>
+        <v>18</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -704,10 +717,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D10" s="3" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -715,10 +728,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>33</v>
+        <v>19</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -726,135 +739,135 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
create scholarships and grade students
</commit_message>
<xml_diff>
--- a/golden heights database/Database Schema.xlsx
+++ b/golden heights database/Database Schema.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\portfolio\portfolio\golden heights database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AAE6E23-8CCF-43D0-A58B-1BD826C3AD99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFAF97CC-39E5-4AD3-9990-012C97495FE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -57,12 +57,6 @@
     <t>Student ID number</t>
   </si>
   <si>
-    <t>Financial aid</t>
-  </si>
-  <si>
-    <t>Financial aid amount</t>
-  </si>
-  <si>
     <t>Degree Type</t>
   </si>
   <si>
@@ -111,9 +105,6 @@
     <t>Grade</t>
   </si>
   <si>
-    <t>Financial Aid</t>
-  </si>
-  <si>
     <t>Enrollment Table(semester-ly)</t>
   </si>
   <si>
@@ -210,9 +201,6 @@
     <t>balance</t>
   </si>
   <si>
-    <t>financial aid</t>
-  </si>
-  <si>
     <t>student(s)</t>
   </si>
   <si>
@@ -220,6 +208,18 @@
   </si>
   <si>
     <t>tuition</t>
+  </si>
+  <si>
+    <t>Scholarships</t>
+  </si>
+  <si>
+    <t>sholarship name</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>scholarship</t>
   </si>
 </sst>
 </file>
@@ -267,14 +267,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,7 +557,7 @@
   <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,15 +575,15 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B1" s="3"/>
       <c r="D1" s="3" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E1" s="3"/>
       <c r="G1" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="H1" s="3"/>
     </row>
@@ -593,19 +592,19 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="G2" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="H2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.3">
@@ -616,16 +615,16 @@
         <v>2</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G3" t="s">
-        <v>10</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
@@ -636,16 +635,16 @@
         <v>3</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="G4" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>63</v>
+        <v>50</v>
+      </c>
+      <c r="G4" t="s">
+        <v>58</v>
+      </c>
+      <c r="H4" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
@@ -653,16 +652,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
+      </c>
+      <c r="H5" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
@@ -670,24 +669,24 @@
         <v>1</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H6" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="H7" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
@@ -695,10 +694,10 @@
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
@@ -706,10 +705,10 @@
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
@@ -717,10 +716,10 @@
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
@@ -728,10 +727,10 @@
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
@@ -739,135 +738,135 @@
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B14" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B17" s="1" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="B24" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>